<commit_message>
Save one scrap on Excel
</commit_message>
<xml_diff>
--- a/list_links_americanas.xlsx
+++ b/list_links_americanas.xlsx
@@ -14,35 +14,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Prices</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>GTX 1650</t>
   </si>
   <si>
     <t>https://www.americanas.com.br/produto/1870191841/placa-de-video-gtx-1650-oc-low-profile-4gb-gddr5-gv-n1650oc-4gl-gibabyte?pfm_carac=gtx%201650&amp;pfm_index=2&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page</t>
   </si>
   <si>
+    <t>https://www.americanas.com.br/produto/1951976949/placa-de-video-gigabyte-nvidia-geforce-gtx-1650-oc-low-profile-gv-n1650oc-4gl?pfm_carac=gtx%201650&amp;pfm_index=4&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page</t>
+  </si>
+  <si>
+    <t>https://www.americanas.com.br/produto/1932205090/placa-de-video-galax-geforce-gtx-1650-ex-4gb-gddr6-1-click-oc-128-bit-65sql8ds66e6?pfm_carac=gtx%201650&amp;pfm_index=6&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page</t>
+  </si>
+  <si>
+    <t>https://www.americanas.com.br/produto/1244339174/placa-de-video-nvidia-geforce-gtx-1650-pegasus-4gb-gddr5-pci-e-3-0-ne51650006g1-1170f-gainward?pfm_carac=gtx%201650&amp;pfm_index=7&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page</t>
+  </si>
+  <si>
     <t>https://www.americanas.com.br/produto/1872858696/placa-de-video-galax-geforce-gtx-1650-1-click-oc-4gb-gddr5-pci-e-3-0-65sql8ds66e6-galax?pfm_carac=gtx%201650&amp;pfm_index=3&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page</t>
   </si>
   <si>
-    <t>https://www.americanas.com.br/produto/1951976949/placa-de-video-gigabyte-nvidia-geforce-gtx-1650-oc-low-profile-gv-n1650oc-4gl?pfm_carac=gtx%201650&amp;pfm_index=4&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page</t>
-  </si>
-  <si>
-    <t>https://www.americanas.com.br/produto/1932205090/placa-de-video-galax-geforce-gtx-1650-ex-4gb-gddr6-1-click-oc-128-bit-65sql8ds66e6?pfm_carac=gtx%201650&amp;pfm_index=6&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page</t>
-  </si>
-  <si>
-    <t>https://www.americanas.com.br/produto/1244339174/placa-de-video-nvidia-geforce-gtx-1650-pegasus-4gb-gddr5-pci-e-3-0-ne51650006g1-1170f-gainward?pfm_carac=gtx%201650&amp;pfm_index=7&amp;pfm_page=search&amp;pfm_pos=grid&amp;pfm_type=search_page</t>
-  </si>
-  <si>
-    <t>GTX 1650</t>
+    <t xml:space="preserve"> 1326,64</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -54,27 +68,6 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -112,23 +105,20 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -431,241 +421,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="20.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="232.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>44064.759093981796</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -677,6 +501,5 @@
     <hyperlink ref="B6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>